<commit_message>
031221 - Dict and misc
</commit_message>
<xml_diff>
--- a/Languages/English/Dictionary.xlsx
+++ b/Languages/English/Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\Tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Github\Self\Hello-World-Of-Everything\Languages\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADC8DAA-533E-4863-AB8A-ECFD0537A1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBB5FC1-E4DF-4A46-BD00-C973E3D71BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{24093F7F-448D-49E3-80AD-727CEF5C7C8D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="304">
   <si>
     <t>intimidating</t>
   </si>
@@ -933,6 +933,21 @@
   </si>
   <si>
     <t>unusual or odd behavior on the part of an individual.</t>
+  </si>
+  <si>
+    <t>incessantly</t>
+  </si>
+  <si>
+    <t>adj</t>
+  </si>
+  <si>
+    <t>without interruption; constantly.</t>
+  </si>
+  <si>
+    <t>she talked about him incessantly</t>
+  </si>
+  <si>
+    <t>endlessly</t>
   </si>
 </sst>
 </file>
@@ -1383,11 +1398,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9A6A0B-6FCC-4EE7-833C-BB640AF8F779}">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
+      <pane ySplit="3" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2571,6 +2586,23 @@
         <v>297</v>
       </c>
     </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D117" t="s">
+        <v>302</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:E90" xr:uid="{2D939F3E-D31B-4C88-978F-943109838C77}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E35">

</xml_diff>

<commit_message>
230709 - Push some misc files for cleaning up
</commit_message>
<xml_diff>
--- a/Languages/English/Dictionary.xlsx
+++ b/Languages/English/Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Github\Self\Hello-World-Of-Everything\Languages\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBB5FC1-E4DF-4A46-BD00-C973E3D71BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C70137-11F0-4612-B238-B3B7411B6C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{24093F7F-448D-49E3-80AD-727CEF5C7C8D}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{24093F7F-448D-49E3-80AD-727CEF5C7C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="352">
   <si>
     <t>intimidating</t>
   </si>
@@ -948,6 +948,186 @@
   </si>
   <si>
     <t>endlessly</t>
+  </si>
+  <si>
+    <t>exasperation</t>
+  </si>
+  <si>
+    <t>a feeling of intense irritation or annoyance.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">she rolled her eyes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in exasperation</t>
+    </r>
+  </si>
+  <si>
+    <t>annoynace, vexation</t>
+  </si>
+  <si>
+    <t>threw up one's hands</t>
+  </si>
+  <si>
+    <t>phrase</t>
+  </si>
+  <si>
+    <t>raise both hands in the air as an indication of one's exasperation.</t>
+  </si>
+  <si>
+    <t>Dickens threw up his hands in impatience</t>
+  </si>
+  <si>
+    <t>perculiar</t>
+  </si>
+  <si>
+    <t>special, strange</t>
+  </si>
+  <si>
+    <t>causality</t>
+  </si>
+  <si>
+    <t>the relationship between cause and effect, the principle that everything has a cause</t>
+  </si>
+  <si>
+    <t>adept</t>
+  </si>
+  <si>
+    <t>very skilled or proficient at something</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">she is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>adept at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cutting through red tape</t>
+    </r>
+  </si>
+  <si>
+    <t>proficient, skillful, talented</t>
+  </si>
+  <si>
+    <t>a person who is skilled or proficient at something</t>
+  </si>
+  <si>
+    <t>he is an adept at imitation</t>
+  </si>
+  <si>
+    <t>expert, master</t>
+  </si>
+  <si>
+    <t>full-fledged</t>
+  </si>
+  <si>
+    <t>completely developed or established</t>
+  </si>
+  <si>
+    <t>implication</t>
+  </si>
+  <si>
+    <t>suggestion, consequence // involvement</t>
+  </si>
+  <si>
+    <t>co-occur</t>
+  </si>
+  <si>
+    <t>occurs together or simultaneously</t>
+  </si>
+  <si>
+    <t>those are the symptoms that always co-occur</t>
+  </si>
+  <si>
+    <t>feeling inferior</t>
+  </si>
+  <si>
+    <t>感到自卑</t>
+  </si>
+  <si>
+    <t>inadequate</t>
+  </si>
+  <si>
+    <t>lacking the quality or quantity required</t>
+  </si>
+  <si>
+    <t>an overwhelming feeling of great happiness or joyful excitement.</t>
+  </si>
+  <si>
+    <t>bliss</t>
+  </si>
+  <si>
+    <t>sceptical</t>
+  </si>
+  <si>
+    <t>not easily convinced</t>
+  </si>
+  <si>
+    <t>ecstatic</t>
+  </si>
+  <si>
+    <t>feeling or expressing overwhelming happiness or joyful excitement</t>
+  </si>
+  <si>
+    <t>ecstatic fans filled the stadium</t>
+  </si>
+  <si>
+    <t>competent</t>
+  </si>
+  <si>
+    <t>having the necessary ability, knowledge, or skill to do something successfully.</t>
+  </si>
+  <si>
+    <t>a highly competent surgeon</t>
+  </si>
+  <si>
+    <t>descrepancy</t>
+  </si>
+  <si>
+    <t>an illogical or surprising lack of compatibility or similarity between two or more facts.</t>
+  </si>
+  <si>
+    <t>there's a discrepancy between your account and his</t>
+  </si>
+  <si>
+    <t>inconsistency, difference, variation</t>
+  </si>
+  <si>
+    <t>emcompass</t>
+  </si>
+  <si>
+    <t>surround and have or hold within.</t>
+  </si>
+  <si>
+    <t>this area of London encompasses Piccadilly to the north and St James's Park to the south</t>
+  </si>
+  <si>
+    <t>includes</t>
   </si>
 </sst>
 </file>
@@ -1034,12 +1214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1051,7 +1231,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1063,23 +1243,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1398,39 +1564,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9A6A0B-6FCC-4EE7-833C-BB640AF8F779}">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E117" sqref="E117"/>
+      <pane ySplit="3" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46" style="14" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="2" width="21.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="46" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="9"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="12"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1440,14 +1606,14 @@
       <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1479,18 +1645,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -1506,7 +1672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -1514,7 +1680,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
@@ -1522,7 +1688,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -1533,23 +1699,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
@@ -1557,7 +1723,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
@@ -1565,7 +1731,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -1573,7 +1739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1581,7 +1747,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1589,7 +1755,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>6</v>
       </c>
@@ -1597,7 +1763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>0</v>
       </c>
@@ -1605,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>56</v>
       </c>
@@ -1613,7 +1779,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
@@ -1621,7 +1787,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
@@ -1629,14 +1795,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1644,7 +1810,7 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
@@ -1652,7 +1818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
@@ -1660,7 +1826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>43</v>
       </c>
@@ -1668,18 +1834,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
@@ -1690,7 +1856,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>54</v>
       </c>
@@ -1698,7 +1864,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
@@ -1706,7 +1872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>62</v>
       </c>
@@ -1714,7 +1880,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
@@ -1722,12 +1888,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>72</v>
       </c>
@@ -1735,62 +1901,62 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>87</v>
       </c>
@@ -1801,21 +1967,21 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>94</v>
       </c>
@@ -1826,7 +1992,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>97</v>
       </c>
@@ -1837,21 +2003,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="2" t="s">
         <v>102</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>104</v>
       </c>
@@ -1862,7 +2028,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>107</v>
       </c>
@@ -1870,54 +2036,54 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>122</v>
       </c>
@@ -1928,18 +2094,18 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>128</v>
       </c>
@@ -1947,74 +2113,74 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>134</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>134</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>140</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="2" t="s">
         <v>143</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>145</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="2" t="s">
         <v>146</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>148</v>
       </c>
@@ -2022,32 +2188,32 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>153</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="2" t="s">
         <v>155</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>157</v>
       </c>
@@ -2055,7 +2221,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>159</v>
       </c>
@@ -2063,7 +2229,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>161</v>
       </c>
@@ -2071,7 +2237,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>163</v>
       </c>
@@ -2082,18 +2248,18 @@
         <v>168</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>164</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>169</v>
       </c>
@@ -2101,40 +2267,40 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>171</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>174</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D75" s="14" t="s">
+      <c r="D75" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>176</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>179</v>
       </c>
@@ -2142,7 +2308,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>181</v>
       </c>
@@ -2150,29 +2316,29 @@
         <v>182</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>183</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>188</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>190</v>
       </c>
@@ -2180,107 +2346,107 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>191</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D82" s="14" t="s">
+      <c r="D82" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>195</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="2" t="s">
         <v>197</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>199</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D84" s="14" t="s">
+      <c r="D84" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>202</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" s="2" t="s">
         <v>204</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>206</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>208</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>211</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" s="2" t="s">
         <v>213</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>216</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>218</v>
       </c>
@@ -2288,40 +2454,40 @@
         <v>219</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="D91" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="8" t="s">
         <v>229</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="8" t="s">
         <v>232</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>226</v>
       </c>
@@ -2332,7 +2498,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>233</v>
       </c>
@@ -2343,18 +2509,18 @@
         <v>235</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>236</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>239</v>
       </c>
@@ -2362,7 +2528,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>241</v>
       </c>
@@ -2370,32 +2536,32 @@
         <v>242</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>243</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" s="2" t="s">
         <v>245</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D100" s="16" t="s">
+      <c r="D100" s="8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>249</v>
       </c>
@@ -2403,62 +2569,62 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>251</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D102" s="14" t="s">
+      <c r="D102" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>254</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="D103" s="16" t="s">
+      <c r="D103" s="8" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>257</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="D104" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D105" s="16" t="s">
+      <c r="D105" s="8" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>261</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="D106" s="16" t="s">
+      <c r="D106" s="8" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>262</v>
       </c>
@@ -2466,127 +2632,127 @@
         <v>263</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C108" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D108" s="16" t="s">
+      <c r="D108" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D109" s="14" t="s">
+      <c r="D109" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>277</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="8" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>281</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="8" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="17" t="s">
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B112" s="17" t="s">
+      <c r="B112" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C112" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D112" s="14" t="s">
+      <c r="D112" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>280</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="8" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>280</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="8" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>283</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="D115" s="14" t="s">
+      <c r="D115" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>296</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="8" t="s">
         <v>298</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>299</v>
       </c>
@@ -2596,11 +2762,246 @@
       <c r="C117" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="8" t="s">
         <v>302</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C122" t="s">
+        <v>317</v>
+      </c>
+      <c r="D122" t="s">
+        <v>318</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C123" t="s">
+        <v>320</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C128" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C129" t="s">
+        <v>334</v>
+      </c>
+      <c r="D129" t="s">
+        <v>197</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C131" t="s">
+        <v>339</v>
+      </c>
+      <c r="D131" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C132" t="s">
+        <v>342</v>
+      </c>
+      <c r="D132" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>